<commit_message>
formatted to add char + before the phone number
</commit_message>
<xml_diff>
--- a/apps/rahat-ui/public/files/cambodia-file.xlsx
+++ b/apps/rahat-ui/public/files/cambodia-file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">Beneficiary Name</t>
   </si>
@@ -65,14 +65,18 @@
   </si>
   <si>
     <t xml:space="preserve">Phone Status*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -140,12 +144,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -166,76 +178,71 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="57.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.5"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>